<commit_message>
db name change updates
</commit_message>
<xml_diff>
--- a/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
+++ b/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Zero_ProjectTemplate\data_ProjectTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\LUX_ProjectTemplate\data_ProjectTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FFE53E-02E8-4815-AF4E-054C475C8E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A6C935-BD0E-43B1-BD7C-C01A89346CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39540" yWindow="1140" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="batteries" sheetId="2" r:id="rId1"/>
@@ -558,9 +558,6 @@
     <t>latitude</t>
   </si>
   <si>
-    <t>default_operation_mode</t>
-  </si>
-  <si>
     <t>contracted_feed_in_capacity_kw</t>
   </si>
   <si>
@@ -607,6 +604,9 @@
   </si>
   <si>
     <t>gridnode_id</t>
+  </si>
+  <si>
+    <t>operation_mode</t>
   </si>
 </sst>
 </file>
@@ -959,7 +959,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -988,55 +988,55 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>2</v>

</xml_diff>